<commit_message>
Updated BOM for new rev
</commit_message>
<xml_diff>
--- a/Project Outputs for NixieClock_Controller/NixieClock_Controller.xlsx
+++ b/Project Outputs for NixieClock_Controller/NixieClock_Controller.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdiro\Desktop\NixieTubeClock\Project Outputs for NixieClock_Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0879010E-A90A-4DDA-A0DC-866A1DC19574}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4AFD2AD2-2293-4951-A49D-1274F49D2143}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="15435" xr2:uid="{4E813705-27C3-4788-81C9-1EECFC6B275B}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="15435" xr2:uid="{DBF31E2B-83A0-428E-A05F-096FA8F4A7DF}"/>
   </bookViews>
   <sheets>
     <sheet name="NixieClock_Controller" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="149">
   <si>
     <t>Line #</t>
   </si>
@@ -261,10 +261,10 @@
     <t>CP-037A-ND</t>
   </si>
   <si>
-    <t>Header 18X2</t>
-  </si>
-  <si>
-    <t>Header, 18-Pin, Dual row</t>
+    <t>Header 7</t>
+  </si>
+  <si>
+    <t>Header, 7-Pin</t>
   </si>
   <si>
     <t>P2</t>
@@ -273,10 +273,10 @@
     <t>Sullins</t>
   </si>
   <si>
-    <t>PPTC182LFBN-RC</t>
-  </si>
-  <si>
-    <t>S7086-ND</t>
+    <t>PPTC071LFBN-RC</t>
+  </si>
+  <si>
+    <t>S7005-ND</t>
   </si>
   <si>
     <t>Header 5</t>
@@ -294,12 +294,6 @@
     <t>2PH1-05-UA</t>
   </si>
   <si>
-    <t>Unknown</t>
-  </si>
-  <si>
-    <t>2057-2PH1-05-UA-ND</t>
-  </si>
-  <si>
     <t>IRF740</t>
   </si>
   <si>
@@ -321,24 +315,6 @@
     <t>IRF740SPBF-ND</t>
   </si>
   <si>
-    <t>A92</t>
-  </si>
-  <si>
-    <t>PNP Bipolar Transistor</t>
-  </si>
-  <si>
-    <t>Q2, Q3</t>
-  </si>
-  <si>
-    <t>ON Semiconductor</t>
-  </si>
-  <si>
-    <t>MMBTA92LT1G</t>
-  </si>
-  <si>
-    <t>MMBTA92LT1GOSCT-ND</t>
-  </si>
-  <si>
     <t>47K</t>
   </si>
   <si>
@@ -411,7 +387,7 @@
     <t>4.7K</t>
   </si>
   <si>
-    <t>R6, R7</t>
+    <t>R6, R7, R12</t>
   </si>
   <si>
     <t>CRCW0805-4K70FKEA</t>
@@ -420,45 +396,6 @@
     <t>541-4.70KCCT-ND</t>
   </si>
   <si>
-    <t>300K</t>
-  </si>
-  <si>
-    <t>R8, R9</t>
-  </si>
-  <si>
-    <t>CRCW0805300KFKEA</t>
-  </si>
-  <si>
-    <t>541-300KCCT-ND</t>
-  </si>
-  <si>
-    <t>10K</t>
-  </si>
-  <si>
-    <t>R10, R11</t>
-  </si>
-  <si>
-    <t>Yageo</t>
-  </si>
-  <si>
-    <t>RC0805-FR-07-10KL</t>
-  </si>
-  <si>
-    <t>311-10.0KCRCT-ND</t>
-  </si>
-  <si>
-    <t>470K</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>CRCW0805470KFKEA</t>
-  </si>
-  <si>
-    <t>541-470KCCT-ND</t>
-  </si>
-  <si>
     <t>SW-PB</t>
   </si>
   <si>
@@ -490,21 +427,6 @@
   </si>
   <si>
     <t>296-11287-5-ND</t>
-  </si>
-  <si>
-    <t>HV5623</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>Microchip Supertex</t>
-  </si>
-  <si>
-    <t>HV5623K7-G</t>
-  </si>
-  <si>
-    <t>HV5623K7-G-ND</t>
   </si>
   <si>
     <t>attiny1617</t>
@@ -934,11 +856,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88969F43-8071-4918-AFD0-0F160782B2D6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A48D6E68-5E7C-428C-8337-FBC7D01E0D0A}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1028,10 +950,10 @@
         <v>20</v>
       </c>
       <c r="K2" s="4">
-        <v>1.75</v>
+        <v>1.66</v>
       </c>
       <c r="L2" s="4">
-        <v>1.75</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1066,10 +988,10 @@
         <v>26</v>
       </c>
       <c r="K3" s="4">
-        <v>0.22647</v>
+        <v>0.21548999999999999</v>
       </c>
       <c r="L3" s="4">
-        <v>0.22647</v>
+        <v>0.21548999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1104,10 +1026,10 @@
         <v>32</v>
       </c>
       <c r="K4" s="4">
-        <v>0.45294000000000001</v>
+        <v>0.43097000000000002</v>
       </c>
       <c r="L4" s="4">
-        <v>0.45294000000000001</v>
+        <v>0.43097000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1142,10 +1064,10 @@
         <v>36</v>
       </c>
       <c r="K5" s="4">
-        <v>0.14654</v>
+        <v>0.13943</v>
       </c>
       <c r="L5" s="4">
-        <v>0.14654</v>
+        <v>0.13943</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1179,12 +1101,8 @@
       <c r="J6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K6" s="4">
-        <v>1.07</v>
-      </c>
-      <c r="L6" s="4">
-        <v>1.07</v>
-      </c>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1218,10 +1136,10 @@
         <v>44</v>
       </c>
       <c r="K7" s="4">
-        <v>0.18651000000000001</v>
+        <v>0.17746000000000001</v>
       </c>
       <c r="L7" s="4">
-        <v>0.37301000000000001</v>
+        <v>0.35492000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1256,14 +1174,16 @@
         <v>48</v>
       </c>
       <c r="K8" s="4">
-        <v>0.23979</v>
+        <v>0.22816</v>
       </c>
       <c r="L8" s="4">
-        <v>1.2</v>
+        <v>1.1399999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+      <c r="A9" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="B9" s="3" t="s">
         <v>49</v>
       </c>
@@ -1292,10 +1212,10 @@
         <v>53</v>
       </c>
       <c r="K9" s="4">
-        <v>0.89256000000000002</v>
+        <v>0.84926999999999997</v>
       </c>
       <c r="L9" s="4">
-        <v>0.89256000000000002</v>
+        <v>0.84926999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1329,12 +1249,8 @@
       <c r="J10" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="K10" s="4">
-        <v>0.67940999999999996</v>
-      </c>
-      <c r="L10" s="4">
-        <v>0.67940999999999996</v>
-      </c>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -1367,12 +1283,8 @@
       <c r="J11" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="K11" s="4">
-        <v>5.99</v>
-      </c>
-      <c r="L11" s="4">
-        <v>17.98</v>
-      </c>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1405,12 +1317,8 @@
       <c r="J12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="K12" s="4">
-        <v>3</v>
-      </c>
-      <c r="L12" s="4">
-        <v>3</v>
-      </c>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -1443,17 +1351,11 @@
       <c r="J13" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K13" s="4">
-        <v>0.77266000000000001</v>
-      </c>
-      <c r="L13" s="4">
-        <v>0.77266000000000001</v>
-      </c>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A14" s="4"/>
       <c r="B14" s="3" t="s">
         <v>77</v>
       </c>
@@ -1482,10 +1384,10 @@
         <v>82</v>
       </c>
       <c r="K14" s="4">
-        <v>2.74</v>
+        <v>0.74787000000000003</v>
       </c>
       <c r="L14" s="4">
-        <v>2.74</v>
+        <v>0.74787000000000003</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1511,95 +1413,83 @@
         <v>87</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="K15" s="4">
-        <v>0.23979</v>
-      </c>
-      <c r="L15" s="4">
-        <v>0.23979</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="E16" s="4">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E16" s="4">
-        <v>1</v>
-      </c>
-      <c r="F16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="I16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="I16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="K16" s="4">
-        <v>2.93</v>
-      </c>
-      <c r="L16" s="4">
-        <v>2.93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="E17" s="4">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="H17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E17" s="4">
-        <v>2</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="K17" s="4">
-        <v>0.23979</v>
+        <v>0.12676000000000001</v>
       </c>
       <c r="L17" s="4">
-        <v>0.47958000000000001</v>
+        <v>0.12676000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1607,37 +1497,37 @@
         <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="H18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E18" s="4">
-        <v>1</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="K18" s="4">
-        <v>0.13322000000000001</v>
+        <v>0.12676000000000001</v>
       </c>
       <c r="L18" s="4">
-        <v>0.13322000000000001</v>
+        <v>0.12676000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1645,37 +1535,37 @@
         <v>12</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E19" s="4">
-        <v>1</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="K19" s="4">
-        <v>0.13322000000000001</v>
+        <v>0.12676000000000001</v>
       </c>
       <c r="L19" s="4">
-        <v>0.13322000000000001</v>
+        <v>0.12676000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1683,113 +1573,113 @@
         <v>12</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="K20" s="4">
+        <v>0.12676000000000001</v>
+      </c>
+      <c r="L20" s="4">
+        <v>0.12676000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D20" s="3" t="s">
+      <c r="C21" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E20" s="4">
-        <v>1</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G20" s="3" t="s">
+      <c r="E21" s="4">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="H20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J20" s="3" t="s">
+      <c r="G21" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="K20" s="4">
-        <v>0.13322000000000001</v>
-      </c>
-      <c r="L20" s="4">
-        <v>0.13322000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="3" t="s">
+      <c r="H21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D21" s="3" t="s">
+      <c r="K21" s="4">
+        <v>0.32956999999999997</v>
+      </c>
+      <c r="L21" s="4">
+        <v>0.32956999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="E21" s="4">
-        <v>1</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G21" s="3" t="s">
+      <c r="C22" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="H21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J21" s="3" t="s">
+      <c r="E22" s="4">
+        <v>3</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="K21" s="4">
-        <v>0.13322000000000001</v>
-      </c>
-      <c r="L21" s="4">
-        <v>0.13322000000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="H22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E22" s="4">
-        <v>1</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="K22" s="4">
-        <v>0.34637000000000001</v>
+        <v>0.12676000000000001</v>
       </c>
       <c r="L22" s="4">
-        <v>0.34637000000000001</v>
+        <v>0.38027</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1797,75 +1687,75 @@
         <v>12</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E23" s="4">
+        <v>3</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="H23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E23" s="4">
-        <v>2</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G23" s="3" t="s">
+      <c r="K23" s="4">
+        <v>0.40561999999999998</v>
+      </c>
+      <c r="L23" s="4">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="H23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J23" s="3" t="s">
+      <c r="C24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="K23" s="4">
-        <v>0.13322000000000001</v>
-      </c>
-      <c r="L23" s="4">
-        <v>0.26644000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="E24" s="4">
+        <v>1</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D24" s="3" t="s">
+      <c r="G24" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E24" s="4">
-        <v>2</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G24" s="3" t="s">
+      <c r="H24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J24" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="H24" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>133</v>
-      </c>
       <c r="K24" s="4">
-        <v>0.13322000000000001</v>
+        <v>1.77</v>
       </c>
       <c r="L24" s="4">
-        <v>0.26644000000000001</v>
+        <v>1.77</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1873,48 +1763,48 @@
         <v>12</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" s="4">
+        <v>1</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E25" s="4">
-        <v>2</v>
-      </c>
-      <c r="F25" s="3" t="s">
+      <c r="G25" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="H25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="H25" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J25" s="3" t="s">
+      <c r="K25" s="4">
+        <v>1.17</v>
+      </c>
+      <c r="L25" s="4">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="K25" s="4">
-        <v>0.13322000000000001</v>
-      </c>
-      <c r="L25" s="4">
-        <v>0.26644000000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>140</v>
@@ -1923,10 +1813,10 @@
         <v>1</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>93</v>
+        <v>141</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>18</v>
@@ -1937,14 +1827,10 @@
       <c r="J26" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="K26" s="4">
-        <v>0.13322000000000001</v>
-      </c>
-      <c r="L26" s="4">
-        <v>0.13322000000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>12</v>
       </c>
@@ -1958,7 +1844,7 @@
         <v>145</v>
       </c>
       <c r="E27" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>146</v>
@@ -1976,198 +1862,10 @@
         <v>148</v>
       </c>
       <c r="K27" s="4">
-        <v>0.42630000000000001</v>
+        <v>0.51970000000000005</v>
       </c>
       <c r="L27" s="4">
-        <v>1.28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="E28" s="4">
-        <v>1</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="K28" s="4">
-        <v>1.87</v>
-      </c>
-      <c r="L28" s="4">
-        <v>1.87</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E29" s="4">
-        <v>1</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="K29" s="4">
-        <v>10.14</v>
-      </c>
-      <c r="L29" s="4">
-        <v>10.14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="E30" s="4">
-        <v>1</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="K30" s="4">
-        <v>1.23</v>
-      </c>
-      <c r="L30" s="4">
-        <v>1.23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="E31" s="4">
-        <v>1</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J31" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="K31" s="4">
-        <v>10.24</v>
-      </c>
-      <c r="L31" s="4">
-        <v>10.24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="E32" s="4">
-        <v>1</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="K32" s="4">
-        <v>0.54618999999999995</v>
-      </c>
-      <c r="L32" s="4">
-        <v>0.54618999999999995</v>
+        <v>0.51970000000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>